<commit_message>
Last updates are done.
</commit_message>
<xml_diff>
--- a/CIV_Ders_Programi_2025_2026.xlsx
+++ b/CIV_Ders_Programi_2025_2026.xlsx
@@ -1,40 +1,200 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enes\Desktop\education\Business Intelligence and Data Mining\idu-program-generator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35401346-8065-449C-919E-71C21F287A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Ders Programı" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
+  <si>
+    <t>Gün</t>
+  </si>
+  <si>
+    <t>Saat</t>
+  </si>
+  <si>
+    <t>1. Sınıf</t>
+  </si>
+  <si>
+    <t>2. Sınıf</t>
+  </si>
+  <si>
+    <t>3. Sınıf</t>
+  </si>
+  <si>
+    <t>4. Sınıf</t>
+  </si>
+  <si>
+    <t>Pazartesi</t>
+  </si>
+  <si>
+    <t>10:20 - 11:05</t>
+  </si>
+  <si>
+    <t>CIV 101 Introduction to Civil Engineering and Ethics (A211)
+Dr. Öğr. Üyesi Ziya ÇAKIÇI</t>
+  </si>
+  <si>
+    <t>11:15 - 12:00</t>
+  </si>
+  <si>
+    <t>13:25 - 14:10</t>
+  </si>
+  <si>
+    <t>CIV 201 Numerical Analysis (C307)
+Doç. Dr. Elif Çağda KANDEMİR</t>
+  </si>
+  <si>
+    <t>14:20 - 15:05</t>
+  </si>
+  <si>
+    <t>CIV 103 Technical Drawing and Computer Aided Engineering Design (A203)
+Dr. Öğr. Üyesi Esra GÜNERİ</t>
+  </si>
+  <si>
+    <t>15:15 - 16:00</t>
+  </si>
+  <si>
+    <t>16:10 - 16:55</t>
+  </si>
+  <si>
+    <t>17:05 - 17:50</t>
+  </si>
+  <si>
+    <t>CIV 103 Technical Drawing and Computer Aided Engineering Design (A209)
+Dr. Öğr. Üyesi Esra GÜNERİ</t>
+  </si>
+  <si>
+    <t>Salı</t>
+  </si>
+  <si>
+    <t>08:30 - 09:15</t>
+  </si>
+  <si>
+    <t>CIV 207 Materials Science (AL06)
+Doç. Dr. Hacı Süleyman GÖKÇE</t>
+  </si>
+  <si>
+    <t>09:25 - 10:10</t>
+  </si>
+  <si>
+    <t>12:30 - 13:15</t>
+  </si>
+  <si>
+    <t>CIV 209 Fluid Mechanics (A209)
+Dr. Öğr. Üyesi Mert Sinan TURGUT</t>
+  </si>
+  <si>
+    <t>CIV 203 Strength of Materials I (A203)
+Doç. Dr. Ali MORTAZAVİ</t>
+  </si>
+  <si>
+    <t>Çarşamba</t>
+  </si>
+  <si>
+    <t>CIV 211 Occupational Health and Safety I (AL06)
+Prof. Dr. Nazife DOĞAN</t>
+  </si>
+  <si>
+    <t>CIV 205 Geology for Civil Engineers (AL06)
+Prof. Dr. Nazife DOĞAN</t>
+  </si>
+  <si>
+    <t>Cuma</t>
+  </si>
+  <si>
+    <t>USEC 235 Latin Dances (AL05)
+Doç. Dr. Hacı Süleyman GÖKÇE</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="162"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD700"/>
+        <bgColor rgb="FFFFD700"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFACD"/>
+        <bgColor rgb="FFFFFACD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -42,85 +202,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,19 +589,345 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="6" width="30" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="4"/>
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6"/>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+    </row>
+    <row r="21" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+    </row>
+    <row r="22" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A18"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A24"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>